<commit_message>
fixes on ml and pst setup
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/particle_tracking/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFA26BC-8AC2-BD4B-9FC0-EC61D42A0266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30733942-5FA0-C045-9218-7A877D37CA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="2140" windowWidth="14520" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -559,7 +559,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="3">
-        <v>1E-4</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
non zero starting mr
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90405F79-409D-C349-94F2-A37E4F67CD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D5B6F9-11F9-6B42-AA47-A49313B9B435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="3360" windowWidth="14520" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8460" yWindow="500" windowWidth="14520" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -559,7 +559,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
replaced N_RIV by H_REF
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E899B6-0FB5-4F45-8064-185FE431EABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470B801-11E3-2B40-BB82-94E1203E144C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="2860" windowWidth="14520" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="500" windowWidth="14520" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -559,7 +559,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="3">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
new pp set and refinement zones
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470B801-11E3-2B40-BB82-94E1203E144C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A48EFC-E700-A646-8AB0-8E4F7AD71183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="500" windowWidth="14520" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -530,8 +530,8 @@
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <f>200/(1000*365*86400)</f>
-        <v>6.3419583967529172E-9</v>
+        <f>300/(1000*365*86400)</f>
+        <v>9.5129375951293758E-9</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
new pilot points and pst fixes
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A409AD2A-0EB3-6046-9AA7-072100C7BF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC7DB0D-4540-EF43-B16C-85A93463D5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12260" yWindow="500" windowWidth="13340" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="23760" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
   <si>
     <t>name</t>
   </si>
@@ -45,12 +45,6 @@
     <t>group</t>
   </si>
   <si>
-    <t>pp_trans</t>
-  </si>
-  <si>
-    <t>pp_sto</t>
-  </si>
-  <si>
     <t>partrans</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>C_BLANC_AMONT</t>
   </si>
   <si>
@@ -178,6 +169,12 @@
   </si>
   <si>
     <t>H_BAR</t>
+  </si>
+  <si>
+    <t>priorlbnd</t>
+  </si>
+  <si>
+    <t>priorubnd</t>
   </si>
 </sst>
 </file>
@@ -511,20 +508,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,34 +532,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="2">
         <f>300/(1000*365*86400)</f>
         <v>9.5129375951293758E-9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3">
         <f>50/(1000*365*86400)</f>
@@ -573,647 +576,729 @@
         <v>1.5854895991882293E-8</v>
       </c>
       <c r="G2" s="3">
+        <f>50/(1000*365*86400)</f>
+        <v>1.5854895991882293E-9</v>
+      </c>
+      <c r="H2" s="3">
+        <f>500/(1000*365*86400)</f>
+        <v>1.5854895991882293E-8</v>
+      </c>
+      <c r="I2" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="H2" s="3">
+      <c r="J2" s="3">
         <v>100000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="3">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F3" s="3">
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="3">
+      <c r="I3" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="J3" s="3">
         <v>100000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F4" s="3">
+        <v>1E-8</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1E-10</v>
+      </c>
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="3">
+      <c r="I4" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="J4" s="3">
         <v>100000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3">
-        <v>1E-10</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="H5" s="3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>1E-3</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>1E-3</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>1E-3</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
         <v>1E-4</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>1E-4</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>1E-4</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>1E-4</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>1E-3</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>1E-3</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>1E-3</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>1E-3</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>1E-3</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>1E-3</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>1E-3</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>1E-3</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>1E-3</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3">
+        <v>1E-8</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G24" s="3">
         <v>1E-10</v>
       </c>
-      <c r="F25" s="3">
+      <c r="H24" s="3">
         <v>1</v>
       </c>
-      <c r="G25" s="3">
+      <c r="I24" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="H25" s="3">
+      <c r="J24" s="3">
         <v>100000</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1">
         <v>1E-3</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="3">
+        <f>AVERAGE(B29:B30)</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3">
+        <v>1E-8</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G27" s="3">
         <v>1E-10</v>
       </c>
-      <c r="F28" s="3">
+      <c r="H27" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="3">
+      <c r="I27" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="H28" s="3">
+      <c r="J27" s="3">
         <v>100000</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29">
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+        <v>4</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="2">
+        <f>AVERAGE(B32)</f>
+        <v>-6.9444444444444448E-2</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="3">
+        <f>G31</f>
+        <v>-0.1388888888888889</v>
+      </c>
+      <c r="F31" s="3">
+        <f>H31</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <f>G32</f>
+        <v>-0.1388888888888889</v>
+      </c>
+      <c r="H31" s="3">
+        <f>H32</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B32" s="4">
         <f>-250/3600</f>
         <v>-6.9444444444444448E-2</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="4">
+        <v>8</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4">
         <f>-500/3600</f>
         <v>-0.1388888888888889</v>
       </c>
-      <c r="F32" s="4">
+      <c r="H32" s="4">
         <v>0</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B33" s="4">
         <f>B32</f>
         <v>-6.9444444444444448E-2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4">
+        <f>G32</f>
+        <v>-0.1388888888888889</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="2">
+        <f>AVERAGE(B35:B36)</f>
+        <v>8.6</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2">
+        <f>G34</f>
+        <v>7</v>
+      </c>
+      <c r="F34" s="2">
+        <f>H34</f>
         <v>10</v>
       </c>
-      <c r="E33" s="4">
-        <f>E32</f>
-        <v>-0.1388888888888889</v>
-      </c>
-      <c r="F33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="4">
+      <c r="G34" s="2">
+        <f>G35</f>
+        <v>7</v>
+      </c>
+      <c r="H34" s="2">
+        <f>H35</f>
+        <v>10</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="4">
         <v>8</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4">
+        <v>7</v>
+      </c>
+      <c r="H35" s="4">
         <v>10</v>
       </c>
-      <c r="E34" s="4">
-        <v>7</v>
-      </c>
-      <c r="F34" s="4">
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="4">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4">
+        <v>9</v>
+      </c>
+      <c r="H36" s="4">
         <v>10</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="4">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="4">
-        <v>9</v>
-      </c>
-      <c r="F35" s="4">
-        <v>10</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
n_part=500, set fac lw and up bnds
</commit_message>
<xml_diff>
--- a/data/par.xlsx
+++ b/data/par.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apryet/recherche/ptrack/case_study/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B11475-216E-D348-92A4-5E63F3AC73A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFE094D-0584-1647-8B22-5F7020011D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1900" windowWidth="23760" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -584,10 +584,10 @@
         <v>1.5854895991882293E-8</v>
       </c>
       <c r="I2" s="3">
-        <v>1.0000000000000001E-5</v>
+        <v>0.01</v>
       </c>
       <c r="J2" s="3">
-        <v>100000</v>
+        <v>100</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -617,10 +617,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="3">
-        <v>1.0000000000000001E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="J3" s="3">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -1018,7 +1018,7 @@
         <v>1E-10</v>
       </c>
       <c r="H24" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I24" s="3">
         <v>1.0000000000000001E-5</v>
@@ -1085,7 +1085,7 @@
         <v>1E-10</v>
       </c>
       <c r="H27" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I27" s="3">
         <v>1.0000000000000001E-5</v>

</xml_diff>